<commit_message>
get credentials from orchestrator done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\MetaMarian_Robot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosmin.oanea\Documents\IS\MetaMarian\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B67866B-C4C6-411C-9AB6-B65203BFA3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9518036-E23D-40E6-BED6-E0FC3C55B80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
+    <sheet name="Credentials" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -163,6 +164,12 @@
   </si>
   <si>
     <t>HRCredentials</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderPath</t>
+  </si>
+  <si>
+    <t>Shared/Metamarian</t>
   </si>
 </sst>
 </file>
@@ -530,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -604,29 +611,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
-      <c r="A5" t="s">
+    <row r="4" spans="1:26" ht="14.5">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="29">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1616,6 +1627,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1627,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2790,7 +2802,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3839,4 +3853,46 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B5FB60-6BC4-4331-9EE7-53A3CF42BA3A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="40.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>